<commit_message>
Updated burn up charts
</commit_message>
<xml_diff>
--- a/docs/Burn Up Charts/Burn Up Chart.xlsx
+++ b/docs/Burn Up Charts/Burn Up Chart.xlsx
@@ -423,11 +423,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124364720"/>
-        <c:axId val="123834992"/>
+        <c:axId val="124320240"/>
+        <c:axId val="153134864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="124364720"/>
+        <c:axId val="124320240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,14 +531,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123834992"/>
+        <c:crossAx val="153134864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="123834992"/>
+        <c:axId val="153134864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124364720"/>
+        <c:crossAx val="124320240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1004,28 +1004,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,11 +1042,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="153777472"/>
-        <c:axId val="121206080"/>
+        <c:axId val="287701184"/>
+        <c:axId val="153600480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="153777472"/>
+        <c:axId val="287701184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,14 +1089,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121206080"/>
+        <c:crossAx val="153600480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="121206080"/>
+        <c:axId val="153600480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1147,7 +1147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153777472"/>
+        <c:crossAx val="287701184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1423,7 +1423,7 @@
                   <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,11 +1552,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="156248400"/>
-        <c:axId val="125012256"/>
+        <c:axId val="156905504"/>
+        <c:axId val="153210080"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="156248400"/>
+        <c:axId val="156905504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1580,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1599,14 +1599,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125012256"/>
+        <c:crossAx val="153210080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="125012256"/>
+        <c:axId val="153210080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1657,7 +1657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156248400"/>
+        <c:crossAx val="156905504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,28 +2179,28 @@
                   <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>66.0</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>31.0</c:v>
@@ -2244,11 +2244,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124204400"/>
-        <c:axId val="156766592"/>
+        <c:axId val="151054784"/>
+        <c:axId val="153176208"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="124204400"/>
+        <c:axId val="151054784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,14 +2347,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156766592"/>
+        <c:crossAx val="153176208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="156766592"/>
+        <c:axId val="153176208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2460,7 +2460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124204400"/>
+        <c:crossAx val="151054784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5145,7 +5145,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5301,7 +5301,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="C9" sqref="A2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5325,7 +5325,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5336,7 +5336,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5347,7 +5347,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5358,7 +5358,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5369,7 +5369,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5380,7 +5380,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5391,7 +5391,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="1">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5402,7 +5402,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="1">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5416,7 +5416,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5528,7 +5528,7 @@
         <v>42697</v>
       </c>
       <c r="B10" s="1">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1">
         <v>31</v>
@@ -5580,7 +5580,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5692,7 +5692,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5703,7 +5703,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5714,7 +5714,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5725,7 +5725,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5736,7 +5736,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5747,7 +5747,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="1">
-        <v>66</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5758,7 +5758,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="1">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5769,7 +5769,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="1">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">

</xml_diff>